<commit_message>
Generate the raw scores in the data preparation
</commit_message>
<xml_diff>
--- a/Questionnaire responses.xlsx
+++ b/Questionnaire responses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kwaku Duah\OneDrive\Documents\R projects\herty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E1A3AA-FAC2-42FE-87F7-9113FB1D2EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B213A3C-BF02-4182-97B0-9A9442115052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="28800" windowHeight="11265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12840" yWindow="2040" windowWidth="28800" windowHeight="11325" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Untitled form" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="80">
   <si>
     <t>15-20</t>
   </si>
@@ -251,6 +251,21 @@
   </si>
   <si>
     <t>section</t>
+  </si>
+  <si>
+    <t>imp_score</t>
+  </si>
+  <si>
+    <t>Score for imposterism</t>
+  </si>
+  <si>
+    <t>pers_score</t>
+  </si>
+  <si>
+    <t>Persistence score</t>
+  </si>
+  <si>
+    <t>eff_score</t>
   </si>
 </sst>
 </file>
@@ -606,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
@@ -8936,10 +8951,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDAEA53-5DC4-49A9-99F6-653526461015}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9224,6 +9239,39 @@
         <v>73</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>